<commit_message>
Primer commit: proyecto OCG_2026
</commit_message>
<xml_diff>
--- a/calendario_guardias_2026.xlsx
+++ b/calendario_guardias_2026.xlsx
@@ -1080,6 +1080,306 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Lun</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Mié</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Jue</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Vie</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Sáb</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Dom</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="G2" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>GUIM TORRES</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GUIM DIAZ</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TN MACHUCA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>GUIM TORRES</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>TF ONETO CAJAL</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>GUIM TORRES</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>TN MACHUCA</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>GUIM DIAZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TN MACHUCA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GUIM DIAZ</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>TN MACHUCA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>TF ONETO CAJAL</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>GUIM DIAZ</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>TF ONETO CAJAL</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>TFCO LEDESMA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TC LEDESMA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TCCO PALMA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>TNIM BUTASSI</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>TC LEDESMA</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>TNIM BUTASSI</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>TF ZALAZAR</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>GUCO BENITEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TCCO PALMA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>TF ZALAZAR</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>TFCO LEDESMA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>GUCO BENITEZ</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>TNIM BUTASSI</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>GUIM DIAZ</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1130,13 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>GUIM TORRES</t>
-        </is>
-      </c>
-    </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" s="3" t="n">
         <v>2</v>
@@ -1163,37 +1457,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GUIM DIAZ</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>TN MACHUCA</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>GUIM TORRES</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>TF ONETO CAJAL</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>GUIM TORRES</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>TN MACHUCA</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>GUIM DIAZ</t>
+          <t>TNIM BUTASSI</t>
         </is>
       </c>
     </row>
@@ -1220,48 +1484,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>TN MACHUCA</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>GUIM DIAZ</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>TN MACHUCA</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>TF ONETO CAJAL</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>GUIM DIAZ</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>TF ONETO CAJAL</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>TFCO LEDESMA</t>
-        </is>
-      </c>
-    </row>
+    <row r="7"/>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="3" t="n">
         <v>17</v>
       </c>
       <c r="C8" s="3" t="n">
@@ -1280,48 +1508,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>TC LEDESMA</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>TCCO PALMA</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>TFCO LEDESMA</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>TC LEDESMA</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>TNIM BUTASSI</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>TF ZALAZAR</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>GUCO BENITEZ</t>
-        </is>
-      </c>
-    </row>
+    <row r="9"/>
     <row r="10">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="1" t="n">
         <v>24</v>
       </c>
       <c r="C10" s="3" t="n">
@@ -1336,40 +1528,19 @@
       <c r="F10" s="1" t="n">
         <v>28</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>TCCO PALMA</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>TF ZALAZAR</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>TNAU BARRIOS</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>GUCO BENITEZ</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>TNIM BUTASSI</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>TNAU BARRIOS</t>
-        </is>
-      </c>
-    </row>
-    <row r="12"/>
+      <c r="G10" s="1" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11"/>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>31</v>
+      </c>
+    </row>
     <row r="13"/>
     <row r="14"/>
     <row r="15"/>
@@ -1412,167 +1583,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Lun</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Mar</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Mié</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Jue</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Vie</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Sáb</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Dom</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="G2" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>18</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>26</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="n">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>